<commit_message>
Added logic for interpreting test image results
</commit_message>
<xml_diff>
--- a/CNN_Misclassifications_Testing.xlsx
+++ b/CNN_Misclassifications_Testing.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -370,7 +370,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>probability_unfriendly</t>
+          <t>predicted_label</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>probability_problematic</t>
         </is>
       </c>
     </row>
@@ -382,10 +387,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C2">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D2">
         <v>5.579540385269866e-08</v>
       </c>
     </row>
@@ -397,10 +407,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C3">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D3">
         <v>1.0137542716393e-07</v>
       </c>
     </row>
@@ -412,10 +427,15 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C4">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D4">
         <v>1.942772200891341e-07</v>
       </c>
     </row>
@@ -427,10 +447,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C5">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D5">
         <v>2.320203265071541e-07</v>
       </c>
     </row>
@@ -442,10 +467,15 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C6">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D6">
         <v>8.667873316881014e-07</v>
       </c>
     </row>
@@ -457,10 +487,15 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C7">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D7">
         <v>1.996663286263356e-06</v>
       </c>
     </row>
@@ -472,10 +507,15 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C8">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D8">
         <v>9.924060577759521e-05</v>
       </c>
     </row>
@@ -487,10 +527,15 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C9">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D9">
         <v>9.996653534471987e-05</v>
       </c>
     </row>
@@ -502,10 +547,15 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C10">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D10">
         <v>0.00027824603603221</v>
       </c>
     </row>
@@ -517,10 +567,15 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C11">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D11">
         <v>0.00030001884442754</v>
       </c>
     </row>
@@ -532,10 +587,15 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C12">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D12">
         <v>0.00050872057909145</v>
       </c>
     </row>
@@ -547,10 +607,15 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C13">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D13">
         <v>0.00056138192303478</v>
       </c>
     </row>
@@ -562,10 +627,15 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C14">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D14">
         <v>0.00057907088194042</v>
       </c>
     </row>
@@ -577,10 +647,15 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C15">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D15">
         <v>0.00060102081624791</v>
       </c>
     </row>
@@ -592,10 +667,15 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C16">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D16">
         <v>0.0006627911934629</v>
       </c>
     </row>
@@ -607,10 +687,15 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C17">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D17">
         <v>0.0009417770197615</v>
       </c>
     </row>
@@ -622,10 +707,15 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C18">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D18">
         <v>0.00212913495488464</v>
       </c>
     </row>
@@ -637,10 +727,15 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C19">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D19">
         <v>0.00286382599733769</v>
       </c>
     </row>
@@ -652,10 +747,15 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C20">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D20">
         <v>0.00432328786700964</v>
       </c>
     </row>
@@ -667,10 +767,15 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C21">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D21">
         <v>0.00464463839307427</v>
       </c>
     </row>
@@ -682,10 +787,15 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C22">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D22">
         <v>0.00521574495360255</v>
       </c>
     </row>
@@ -697,10 +807,15 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C23">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D23">
         <v>0.00607008673250675</v>
       </c>
     </row>
@@ -712,10 +827,15 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C24">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D24">
         <v>0.00719824759289622</v>
       </c>
     </row>
@@ -727,10 +847,15 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C25">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D25">
         <v>0.01353177335113287</v>
       </c>
     </row>
@@ -742,10 +867,15 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C26">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D26">
         <v>0.01430556271225214</v>
       </c>
     </row>
@@ -757,10 +887,15 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C27">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D27">
         <v>0.01506472285836935</v>
       </c>
     </row>
@@ -772,10 +907,15 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C28">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D28">
         <v>0.02072608843445778</v>
       </c>
     </row>
@@ -787,10 +927,15 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C29">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D29">
         <v>0.02515900507569313</v>
       </c>
     </row>
@@ -802,10 +947,15 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C30">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D30">
         <v>0.03448681160807609</v>
       </c>
     </row>
@@ -817,10 +967,15 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C31">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D31">
         <v>0.03505422919988632</v>
       </c>
     </row>
@@ -832,10 +987,15 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C32">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D32">
         <v>0.03699976950883865</v>
       </c>
     </row>
@@ -847,10 +1007,15 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C33">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D33">
         <v>0.04233119264245033</v>
       </c>
     </row>
@@ -862,10 +1027,15 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C34">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D34">
         <v>0.04510199278593063</v>
       </c>
     </row>
@@ -877,10 +1047,15 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C35">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D35">
         <v>0.06024244427680969</v>
       </c>
     </row>
@@ -892,10 +1067,15 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C36">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D36">
         <v>0.06041330099105835</v>
       </c>
     </row>
@@ -907,10 +1087,15 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C37">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D37">
         <v>0.097939632833004</v>
       </c>
     </row>
@@ -922,10 +1107,15 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C38">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D38">
         <v>0.1013156250119209</v>
       </c>
     </row>
@@ -937,10 +1127,15 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C39">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D39">
         <v>0.1493371725082398</v>
       </c>
     </row>
@@ -952,10 +1147,15 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C40">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D40">
         <v>0.1528811901807785</v>
       </c>
     </row>
@@ -967,10 +1167,15 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C41">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D41">
         <v>0.2120499610900879</v>
       </c>
     </row>
@@ -982,10 +1187,15 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C42">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D42">
         <v>0.2298745661973953</v>
       </c>
     </row>
@@ -997,10 +1207,15 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C43">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D43">
         <v>0.2756510674953461</v>
       </c>
     </row>
@@ -1012,10 +1227,15 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C44">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D44">
         <v>0.3057629764080048</v>
       </c>
     </row>
@@ -1027,10 +1247,15 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C45">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D45">
         <v>0.3257557451725006</v>
       </c>
     </row>
@@ -1042,10 +1267,15 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C46">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D46">
         <v>0.3445528149604797</v>
       </c>
     </row>
@@ -1057,10 +1287,15 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C47">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D47">
         <v>0.3882490992546082</v>
       </c>
     </row>
@@ -1072,10 +1307,15 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C48">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D48">
         <v>0.4241705238819122</v>
       </c>
     </row>
@@ -1087,10 +1327,15 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C49">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D49">
         <v>0.4267779290676117</v>
       </c>
     </row>
@@ -1102,10 +1347,15 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>unfriendly</t>
-        </is>
-      </c>
-      <c r="C50">
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="D50">
         <v>0.4830842912197113</v>
       </c>
     </row>
@@ -1117,10 +1367,15 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C51">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D51">
         <v>0.9999955296516418</v>
       </c>
     </row>
@@ -1132,10 +1387,15 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C52">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D52">
         <v>0.9999931454658508</v>
       </c>
     </row>
@@ -1147,10 +1407,15 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C53">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D53">
         <v>0.9997333884239196</v>
       </c>
     </row>
@@ -1162,10 +1427,15 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C54">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D54">
         <v>0.9996947646141052</v>
       </c>
     </row>
@@ -1177,10 +1447,15 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C55">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D55">
         <v>0.9985077381134032</v>
       </c>
     </row>
@@ -1192,10 +1467,15 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C56">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D56">
         <v>0.9977074861526488</v>
       </c>
     </row>
@@ -1207,10 +1487,15 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C57">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D57">
         <v>0.991838276386261</v>
       </c>
     </row>
@@ -1222,10 +1507,15 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C58">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D58">
         <v>0.9880274534225464</v>
       </c>
     </row>
@@ -1237,10 +1527,15 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C59">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D59">
         <v>0.9864150285720824</v>
       </c>
     </row>
@@ -1252,10 +1547,15 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C60">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D60">
         <v>0.9861440062522888</v>
       </c>
     </row>
@@ -1267,10 +1567,15 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C61">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D61">
         <v>0.9834773540496826</v>
       </c>
     </row>
@@ -1282,10 +1587,15 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C62">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D62">
         <v>0.9756643176078796</v>
       </c>
     </row>
@@ -1297,10 +1607,15 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C63">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D63">
         <v>0.9747123122215272</v>
       </c>
     </row>
@@ -1312,10 +1627,15 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C64">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D64">
         <v>0.9643343687057496</v>
       </c>
     </row>
@@ -1327,10 +1647,15 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C65">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D65">
         <v>0.9621748924255372</v>
       </c>
     </row>
@@ -1342,10 +1667,15 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C66">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D66">
         <v>0.955525815486908</v>
       </c>
     </row>
@@ -1357,10 +1687,15 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C67">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D67">
         <v>0.9222221970558168</v>
       </c>
     </row>
@@ -1372,10 +1707,15 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C68">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D68">
         <v>0.9156210422515868</v>
       </c>
     </row>
@@ -1387,10 +1727,15 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C69">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D69">
         <v>0.8830835819244385</v>
       </c>
     </row>
@@ -1402,10 +1747,15 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C70">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D70">
         <v>0.8713608980178833</v>
       </c>
     </row>
@@ -1417,10 +1767,15 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C71">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D71">
         <v>0.86494380235672</v>
       </c>
     </row>
@@ -1432,10 +1787,15 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C72">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D72">
         <v>0.7922247648239136</v>
       </c>
     </row>
@@ -1447,10 +1807,15 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C73">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D73">
         <v>0.7693438529968262</v>
       </c>
     </row>
@@ -1462,10 +1827,15 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C74">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D74">
         <v>0.7658854722976685</v>
       </c>
     </row>
@@ -1477,10 +1847,15 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C75">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D75">
         <v>0.7387270331382751</v>
       </c>
     </row>
@@ -1492,10 +1867,15 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C76">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D76">
         <v>0.7274333834648132</v>
       </c>
     </row>
@@ -1507,10 +1887,15 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C77">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D77">
         <v>0.7065933346748352</v>
       </c>
     </row>
@@ -1522,10 +1907,15 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C78">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D78">
         <v>0.6949161887168884</v>
       </c>
     </row>
@@ -1537,10 +1927,15 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C79">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D79">
         <v>0.6794953942298889</v>
       </c>
     </row>
@@ -1552,10 +1947,15 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C80">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D80">
         <v>0.6672936081886292</v>
       </c>
     </row>
@@ -1567,10 +1967,15 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C81">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D81">
         <v>0.6585378646850586</v>
       </c>
     </row>
@@ -1582,10 +1987,15 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C82">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D82">
         <v>0.6561595797538757</v>
       </c>
     </row>
@@ -1597,10 +2007,15 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C83">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D83">
         <v>0.648252546787262</v>
       </c>
     </row>
@@ -1612,10 +2027,15 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C84">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D84">
         <v>0.6268699765205383</v>
       </c>
     </row>
@@ -1627,10 +2047,15 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C85">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D85">
         <v>0.6210244297981262</v>
       </c>
     </row>
@@ -1642,10 +2067,15 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C86">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D86">
         <v>0.6200974583625793</v>
       </c>
     </row>
@@ -1657,10 +2087,15 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C87">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D87">
         <v>0.6130337715148926</v>
       </c>
     </row>
@@ -1672,10 +2107,15 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C88">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D88">
         <v>0.6069692373275757</v>
       </c>
     </row>
@@ -1687,10 +2127,15 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C89">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D89">
         <v>0.6028397083282471</v>
       </c>
     </row>
@@ -1702,10 +2147,15 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C90">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D90">
         <v>0.5725511312484741</v>
       </c>
     </row>
@@ -1717,10 +2167,15 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C91">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D91">
         <v>0.5699270367622375</v>
       </c>
     </row>
@@ -1732,10 +2187,15 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C92">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D92">
         <v>0.5602006316184998</v>
       </c>
     </row>
@@ -1747,10 +2207,15 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>friendly</t>
-        </is>
-      </c>
-      <c r="C93">
+          <t>Definitely okay</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Definitely problematic</t>
+        </is>
+      </c>
+      <c r="D93">
         <v>0.5399845242500305</v>
       </c>
     </row>

</xml_diff>